<commit_message>
Add Branch to sales reports
</commit_message>
<xml_diff>
--- a/public/ExcelTemplates/SalesReportCompact.xlsx
+++ b/public/ExcelTemplates/SalesReportCompact.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.fayez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.fayez\Documents\SalesReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFDABC9-97AB-434F-9A4D-1C19869AA88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0740080-E99B-46BD-AC51-920554E8D680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="المبيعات" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">المبيعات!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">المبيعات!$A$1:$P$1</definedName>
     <definedName name="الاجمالي">المبيعات!#REF!</definedName>
     <definedName name="الشهر">المبيعات!#REF!</definedName>
     <definedName name="الشهر_2">#REF!</definedName>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>م</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>الضريبة</t>
+  </si>
+  <si>
+    <t>الفرع</t>
   </si>
 </sst>
 </file>
@@ -562,11 +565,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -575,21 +578,22 @@
     <col min="2" max="2" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="5"/>
+    <col min="5" max="5" width="10.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,43 +606,46 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A1:O1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:P1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.70866141732282995" right="0.70866141732282995" top="0.74803149606299002" bottom="0.74803149606299002" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" orientation="landscape"/>
 </worksheet>

</xml_diff>